<commit_message>
Thực Hành tuần 2( chỉnh sửa)
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThienNguyen\Documents\GitHub\phattrienungdung\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20025" windowHeight="7875" activeTab="1"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Tasks</t>
   </si>
@@ -155,7 +150,13 @@
     <t>Code Controller</t>
   </si>
   <si>
-    <t>Complete</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Not started</t>
   </si>
 </sst>
 </file>
@@ -365,7 +366,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,7 +401,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,10 +618,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.375" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -831,16 +832,16 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="23.75" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,7 +940,9 @@
       <c r="E5" s="8">
         <v>15</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -957,7 +960,9 @@
       <c r="E6" s="8">
         <v>17</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -975,7 +980,9 @@
       <c r="E7" s="8">
         <v>15</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -993,7 +1000,9 @@
       <c r="E8" s="8">
         <v>20</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -1011,7 +1020,9 @@
       <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1029,7 +1040,9 @@
       <c r="E10" s="8">
         <v>4</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">

</xml_diff>